<commit_message>
Upload File Name and Path Changes
</commit_message>
<xml_diff>
--- a/Test Data/ImportUser_Template.xlsx
+++ b/Test Data/ImportUser_Template.xlsx
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="98">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -320,21 +320,6 @@
     <t xml:space="preserve">Automation User 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Matt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Demon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mat.demon@webspiders.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation User 4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nat</t>
   </si>
   <si>
@@ -350,45 +335,33 @@
     <t xml:space="preserve">Automation User 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Bruce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wills</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brucewills@yopmail.com</t>
+    <t xml:space="preserve">Canon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">canonball@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation User 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zianzay@yopmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">SE</t>
   </si>
   <si>
-    <t xml:space="preserve">Automation User 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ball</t>
-  </si>
-  <si>
-    <t xml:space="preserve">canonball@yopmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation User 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zianzay@yopmail.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Automation User 8</t>
   </si>
   <si>
@@ -405,21 +378,6 @@
   </si>
   <si>
     <t xml:space="preserve">Automation User 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tim.cook@webspiders.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automation User 10</t>
   </si>
   <si>
     <t xml:space="preserve">Phill</t>
@@ -810,24 +768,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.58"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.06"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
@@ -986,20 +944,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="0" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="0" t="s">
@@ -1015,7 +973,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>41</v>
       </c>
@@ -1084,7 +1042,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>16</v>
@@ -1113,13 +1071,13 @@
         <v>57</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>59</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>18</v>
@@ -1133,22 +1091,22 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="E11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>18</v>
@@ -1162,16 +1120,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>16</v>
@@ -1200,13 +1158,13 @@
         <v>71</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>16</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J13" s="7" t="s">
         <v>18</v>
@@ -1220,22 +1178,22 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>16</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J14" s="7" t="s">
         <v>18</v>
@@ -1249,16 +1207,16 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>16</v>
@@ -1345,13 +1303,13 @@
         <v>95</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J18" s="7" t="s">
         <v>18</v>
@@ -1363,93 +1321,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId2" display="adam.smith@webspiders.com"/>
@@ -1464,74 +1338,62 @@
     <hyperlink ref="J4" r:id="rId11" display="https://facebook.com"/>
     <hyperlink ref="K4" r:id="rId12" display="https://twitter.com"/>
     <hyperlink ref="L4" r:id="rId13" display="https://linkedin.com"/>
-    <hyperlink ref="C5" r:id="rId14" display="mat.demon@webspiders.com"/>
+    <hyperlink ref="C5" r:id="rId14" display="nat.gas@webspiders.com"/>
     <hyperlink ref="J5" r:id="rId15" display="https://facebook.com"/>
     <hyperlink ref="K5" r:id="rId16" display="https://twitter.com"/>
     <hyperlink ref="L5" r:id="rId17" display="https://linkedin.com"/>
-    <hyperlink ref="C6" r:id="rId18" display="nat.gas@webspiders.com"/>
+    <hyperlink ref="C6" r:id="rId18" display="canonball@yopmail.com"/>
     <hyperlink ref="J6" r:id="rId19" display="https://facebook.com"/>
     <hyperlink ref="K6" r:id="rId20" display="https://twitter.com"/>
     <hyperlink ref="L6" r:id="rId21" display="https://linkedin.com"/>
-    <hyperlink ref="C7" r:id="rId22" display="brucewills@yopmail.com"/>
+    <hyperlink ref="C7" r:id="rId22" display="zianzay@yopmail.com"/>
     <hyperlink ref="J7" r:id="rId23" display="https://facebook.com"/>
     <hyperlink ref="K7" r:id="rId24" display="https://twitter.com"/>
     <hyperlink ref="L7" r:id="rId25" display="https://linkedin.com"/>
-    <hyperlink ref="C8" r:id="rId26" display="canonball@yopmail.com"/>
+    <hyperlink ref="C8" r:id="rId26" display="gamora.bell@webspiders.com"/>
     <hyperlink ref="J8" r:id="rId27" display="https://facebook.com"/>
     <hyperlink ref="K8" r:id="rId28" display="https://twitter.com"/>
     <hyperlink ref="L8" r:id="rId29" display="https://linkedin.com"/>
-    <hyperlink ref="C9" r:id="rId30" display="zianzay@yopmail.com"/>
+    <hyperlink ref="C9" r:id="rId30" display="phil.moree@webspiders.com"/>
     <hyperlink ref="J9" r:id="rId31" display="https://facebook.com"/>
     <hyperlink ref="K9" r:id="rId32" display="https://twitter.com"/>
     <hyperlink ref="L9" r:id="rId33" display="https://linkedin.com"/>
-    <hyperlink ref="C10" r:id="rId34" display="gamora.bell@webspiders.com"/>
+    <hyperlink ref="C10" r:id="rId34" display="ariya.stark@webspiders.com"/>
     <hyperlink ref="J10" r:id="rId35" display="https://facebook.com"/>
     <hyperlink ref="K10" r:id="rId36" display="https://twitter.com"/>
     <hyperlink ref="L10" r:id="rId37" display="https://linkedin.com"/>
-    <hyperlink ref="C11" r:id="rId38" display="tim.cook@webspiders.com"/>
+    <hyperlink ref="C11" r:id="rId38" display="sam.biz@webspiders.com"/>
     <hyperlink ref="J11" r:id="rId39" display="https://facebook.com"/>
     <hyperlink ref="K11" r:id="rId40" display="https://twitter.com"/>
     <hyperlink ref="L11" r:id="rId41" display="https://linkedin.com"/>
-    <hyperlink ref="C12" r:id="rId42" display="phil.moree@webspiders.com"/>
+    <hyperlink ref="C12" r:id="rId42" display="venu.gopal@webspiders.com"/>
     <hyperlink ref="J12" r:id="rId43" display="https://facebook.com"/>
     <hyperlink ref="K12" r:id="rId44" display="https://twitter.com"/>
     <hyperlink ref="L12" r:id="rId45" display="https://linkedin.com"/>
-    <hyperlink ref="C13" r:id="rId46" display="ariya.stark@webspiders.com"/>
+    <hyperlink ref="C13" r:id="rId46" display="anie.das@webspiders.com"/>
     <hyperlink ref="J13" r:id="rId47" display="https://facebook.com"/>
     <hyperlink ref="K13" r:id="rId48" display="https://twitter.com"/>
     <hyperlink ref="L13" r:id="rId49" display="https://linkedin.com"/>
-    <hyperlink ref="C14" r:id="rId50" display="sam.biz@webspiders.com"/>
+    <hyperlink ref="C14" r:id="rId50" display="miz.maf@webspiders.com"/>
     <hyperlink ref="J14" r:id="rId51" display="https://facebook.com"/>
     <hyperlink ref="K14" r:id="rId52" display="https://twitter.com"/>
     <hyperlink ref="L14" r:id="rId53" display="https://linkedin.com"/>
-    <hyperlink ref="C15" r:id="rId54" display="venu.gopal@webspiders.com"/>
+    <hyperlink ref="C15" r:id="rId54" display="ana.dev@webspiders.com"/>
     <hyperlink ref="J15" r:id="rId55" display="https://facebook.com"/>
     <hyperlink ref="K15" r:id="rId56" display="https://twitter.com"/>
     <hyperlink ref="L15" r:id="rId57" display="https://linkedin.com"/>
-    <hyperlink ref="C16" r:id="rId58" display="anie.das@webspiders.com"/>
+    <hyperlink ref="C16" r:id="rId58" display="khal.kat@webspiders.com"/>
     <hyperlink ref="J16" r:id="rId59" display="https://facebook.com"/>
     <hyperlink ref="K16" r:id="rId60" display="https://twitter.com"/>
     <hyperlink ref="L16" r:id="rId61" display="https://linkedin.com"/>
-    <hyperlink ref="C17" r:id="rId62" display="miz.maf@webspiders.com"/>
+    <hyperlink ref="C17" r:id="rId62" display="jit.singh@webspiders.com"/>
     <hyperlink ref="J17" r:id="rId63" display="https://facebook.com"/>
     <hyperlink ref="K17" r:id="rId64" display="https://twitter.com"/>
     <hyperlink ref="L17" r:id="rId65" display="https://linkedin.com"/>
-    <hyperlink ref="C18" r:id="rId66" display="ana.dev@webspiders.com"/>
+    <hyperlink ref="C18" r:id="rId66" display="ananya.ford@webspiders.com"/>
     <hyperlink ref="J18" r:id="rId67" display="https://facebook.com"/>
     <hyperlink ref="K18" r:id="rId68" display="https://twitter.com"/>
     <hyperlink ref="L18" r:id="rId69" display="https://linkedin.com"/>
-    <hyperlink ref="C19" r:id="rId70" display="khal.kat@webspiders.com"/>
-    <hyperlink ref="J19" r:id="rId71" display="https://facebook.com"/>
-    <hyperlink ref="K19" r:id="rId72" display="https://twitter.com"/>
-    <hyperlink ref="L19" r:id="rId73" display="https://linkedin.com"/>
-    <hyperlink ref="C20" r:id="rId74" display="jit.singh@webspiders.com"/>
-    <hyperlink ref="J20" r:id="rId75" display="https://facebook.com"/>
-    <hyperlink ref="K20" r:id="rId76" display="https://twitter.com"/>
-    <hyperlink ref="L20" r:id="rId77" display="https://linkedin.com"/>
-    <hyperlink ref="C21" r:id="rId78" display="ananya.ford@webspiders.com"/>
-    <hyperlink ref="J21" r:id="rId79" display="https://facebook.com"/>
-    <hyperlink ref="K21" r:id="rId80" display="https://twitter.com"/>
-    <hyperlink ref="L21" r:id="rId81" display="https://linkedin.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1540,6 +1402,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId82"/>
+  <legacyDrawing r:id="rId70"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
True Value CR for Resources Changes Added
</commit_message>
<xml_diff>
--- a/Test Data/ImportUser_Template.xlsx
+++ b/Test Data/ImportUser_Template.xlsx
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="103">
   <si>
     <t xml:space="preserve">FirstName</t>
   </si>
@@ -318,6 +318,21 @@
   </si>
   <si>
     <t xml:space="preserve">Automation User 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bruce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brucewills@yopmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automation User 4</t>
   </si>
   <si>
     <t xml:space="preserve">Nat</t>
@@ -771,7 +786,7 @@
   <dimension ref="A1:L1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -781,7 +796,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.33"/>
@@ -944,20 +959,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="0" t="s">
@@ -1042,13 +1057,13 @@
         <v>53</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>18</v>
@@ -1062,22 +1077,22 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>18</v>
@@ -1091,16 +1106,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>16</v>
@@ -1216,13 +1231,13 @@
         <v>81</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>18</v>
@@ -1236,16 +1251,16 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>16</v>
@@ -1321,7 +1336,35 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1338,62 +1381,66 @@
     <hyperlink ref="J4" r:id="rId11" display="https://facebook.com"/>
     <hyperlink ref="K4" r:id="rId12" display="https://twitter.com"/>
     <hyperlink ref="L4" r:id="rId13" display="https://linkedin.com"/>
-    <hyperlink ref="C5" r:id="rId14" display="nat.gas@webspiders.com"/>
+    <hyperlink ref="C5" r:id="rId14" display="brucewills@yopmail.com"/>
     <hyperlink ref="J5" r:id="rId15" display="https://facebook.com"/>
     <hyperlink ref="K5" r:id="rId16" display="https://twitter.com"/>
     <hyperlink ref="L5" r:id="rId17" display="https://linkedin.com"/>
-    <hyperlink ref="C6" r:id="rId18" display="canonball@yopmail.com"/>
+    <hyperlink ref="C6" r:id="rId18" display="nat.gas@webspiders.com"/>
     <hyperlink ref="J6" r:id="rId19" display="https://facebook.com"/>
     <hyperlink ref="K6" r:id="rId20" display="https://twitter.com"/>
     <hyperlink ref="L6" r:id="rId21" display="https://linkedin.com"/>
-    <hyperlink ref="C7" r:id="rId22" display="zianzay@yopmail.com"/>
+    <hyperlink ref="C7" r:id="rId22" display="canonball@yopmail.com"/>
     <hyperlink ref="J7" r:id="rId23" display="https://facebook.com"/>
     <hyperlink ref="K7" r:id="rId24" display="https://twitter.com"/>
     <hyperlink ref="L7" r:id="rId25" display="https://linkedin.com"/>
-    <hyperlink ref="C8" r:id="rId26" display="gamora.bell@webspiders.com"/>
+    <hyperlink ref="C8" r:id="rId26" display="zianzay@yopmail.com"/>
     <hyperlink ref="J8" r:id="rId27" display="https://facebook.com"/>
     <hyperlink ref="K8" r:id="rId28" display="https://twitter.com"/>
     <hyperlink ref="L8" r:id="rId29" display="https://linkedin.com"/>
-    <hyperlink ref="C9" r:id="rId30" display="phil.moree@webspiders.com"/>
+    <hyperlink ref="C9" r:id="rId30" display="gamora.bell@webspiders.com"/>
     <hyperlink ref="J9" r:id="rId31" display="https://facebook.com"/>
     <hyperlink ref="K9" r:id="rId32" display="https://twitter.com"/>
     <hyperlink ref="L9" r:id="rId33" display="https://linkedin.com"/>
-    <hyperlink ref="C10" r:id="rId34" display="ariya.stark@webspiders.com"/>
+    <hyperlink ref="C10" r:id="rId34" display="phil.moree@webspiders.com"/>
     <hyperlink ref="J10" r:id="rId35" display="https://facebook.com"/>
     <hyperlink ref="K10" r:id="rId36" display="https://twitter.com"/>
     <hyperlink ref="L10" r:id="rId37" display="https://linkedin.com"/>
-    <hyperlink ref="C11" r:id="rId38" display="sam.biz@webspiders.com"/>
+    <hyperlink ref="C11" r:id="rId38" display="ariya.stark@webspiders.com"/>
     <hyperlink ref="J11" r:id="rId39" display="https://facebook.com"/>
     <hyperlink ref="K11" r:id="rId40" display="https://twitter.com"/>
     <hyperlink ref="L11" r:id="rId41" display="https://linkedin.com"/>
-    <hyperlink ref="C12" r:id="rId42" display="venu.gopal@webspiders.com"/>
+    <hyperlink ref="C12" r:id="rId42" display="sam.biz@webspiders.com"/>
     <hyperlink ref="J12" r:id="rId43" display="https://facebook.com"/>
     <hyperlink ref="K12" r:id="rId44" display="https://twitter.com"/>
     <hyperlink ref="L12" r:id="rId45" display="https://linkedin.com"/>
-    <hyperlink ref="C13" r:id="rId46" display="anie.das@webspiders.com"/>
+    <hyperlink ref="C13" r:id="rId46" display="venu.gopal@webspiders.com"/>
     <hyperlink ref="J13" r:id="rId47" display="https://facebook.com"/>
     <hyperlink ref="K13" r:id="rId48" display="https://twitter.com"/>
     <hyperlink ref="L13" r:id="rId49" display="https://linkedin.com"/>
-    <hyperlink ref="C14" r:id="rId50" display="miz.maf@webspiders.com"/>
+    <hyperlink ref="C14" r:id="rId50" display="anie.das@webspiders.com"/>
     <hyperlink ref="J14" r:id="rId51" display="https://facebook.com"/>
     <hyperlink ref="K14" r:id="rId52" display="https://twitter.com"/>
     <hyperlink ref="L14" r:id="rId53" display="https://linkedin.com"/>
-    <hyperlink ref="C15" r:id="rId54" display="ana.dev@webspiders.com"/>
+    <hyperlink ref="C15" r:id="rId54" display="miz.maf@webspiders.com"/>
     <hyperlink ref="J15" r:id="rId55" display="https://facebook.com"/>
     <hyperlink ref="K15" r:id="rId56" display="https://twitter.com"/>
     <hyperlink ref="L15" r:id="rId57" display="https://linkedin.com"/>
-    <hyperlink ref="C16" r:id="rId58" display="khal.kat@webspiders.com"/>
+    <hyperlink ref="C16" r:id="rId58" display="ana.dev@webspiders.com"/>
     <hyperlink ref="J16" r:id="rId59" display="https://facebook.com"/>
     <hyperlink ref="K16" r:id="rId60" display="https://twitter.com"/>
     <hyperlink ref="L16" r:id="rId61" display="https://linkedin.com"/>
-    <hyperlink ref="C17" r:id="rId62" display="jit.singh@webspiders.com"/>
+    <hyperlink ref="C17" r:id="rId62" display="khal.kat@webspiders.com"/>
     <hyperlink ref="J17" r:id="rId63" display="https://facebook.com"/>
     <hyperlink ref="K17" r:id="rId64" display="https://twitter.com"/>
     <hyperlink ref="L17" r:id="rId65" display="https://linkedin.com"/>
-    <hyperlink ref="C18" r:id="rId66" display="ananya.ford@webspiders.com"/>
+    <hyperlink ref="C18" r:id="rId66" display="jit.singh@webspiders.com"/>
     <hyperlink ref="J18" r:id="rId67" display="https://facebook.com"/>
     <hyperlink ref="K18" r:id="rId68" display="https://twitter.com"/>
     <hyperlink ref="L18" r:id="rId69" display="https://linkedin.com"/>
+    <hyperlink ref="C19" r:id="rId70" display="ananya.ford@webspiders.com"/>
+    <hyperlink ref="J19" r:id="rId71" display="https://facebook.com"/>
+    <hyperlink ref="K19" r:id="rId72" display="https://twitter.com"/>
+    <hyperlink ref="L19" r:id="rId73" display="https://linkedin.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1402,6 +1449,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId70"/>
+  <legacyDrawing r:id="rId74"/>
 </worksheet>
 </file>
</xml_diff>